<commit_message>
Replace water with ROR in input data
</commit_message>
<xml_diff>
--- a/raw_data_input/renewables/Prognos_et_al_2020_RES_data.xlsx
+++ b/raw_data_input/renewables/Prognos_et_al_2020_RES_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20378"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yannick\Desktop\SMM\Main\data\Inputlisten\renewables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\koch_j0\POMMES_public\pommes-data\raw_data_input\renewables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98A44323-A681-4D83-8BED-89FFBFDEEAED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A0F28E0-F665-4E55-A1EF-4D11C9AF3C71}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5D64F573-EFB4-433D-A285-0A55FC20DE65}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" xr2:uid="{5D64F573-EFB4-433D-A285-0A55FC20DE65}"/>
   </bookViews>
   <sheets>
     <sheet name="capacities" sheetId="1" r:id="rId1"/>
@@ -21,20 +21,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="11">
   <si>
     <t>fuel</t>
   </si>
@@ -64,6 +56,9 @@
   </si>
   <si>
     <t>biomassEEG</t>
+  </si>
+  <si>
+    <t>ROR</t>
   </si>
 </sst>
 </file>
@@ -417,17 +412,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0A2FDDD-6AA1-45F0-8A84-10A78F9A5494}">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -438,7 +433,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -449,7 +444,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -460,7 +455,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -471,7 +466,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -482,7 +477,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -493,7 +488,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -504,7 +499,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -515,7 +510,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -526,7 +521,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -537,7 +532,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -548,7 +543,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -559,7 +554,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -570,7 +565,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -581,7 +576,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -592,7 +587,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -603,7 +598,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -614,7 +609,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -625,7 +620,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -636,7 +631,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>5</v>
       </c>
@@ -647,7 +642,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>5</v>
       </c>
@@ -658,7 +653,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>5</v>
       </c>
@@ -669,9 +664,9 @@
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B23">
         <v>2018</v>
@@ -680,9 +675,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B24">
         <v>2025</v>
@@ -691,9 +686,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B25">
         <v>2030</v>
@@ -702,9 +697,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B26">
         <v>2035</v>
@@ -713,9 +708,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B27">
         <v>2040</v>
@@ -724,9 +719,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B28">
         <v>2045</v>
@@ -735,9 +730,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B29">
         <v>2050</v>
@@ -746,7 +741,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>9</v>
       </c>
@@ -757,7 +752,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>9</v>
       </c>
@@ -768,7 +763,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>9</v>
       </c>
@@ -779,7 +774,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>9</v>
       </c>
@@ -790,7 +785,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>9</v>
       </c>
@@ -801,7 +796,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>9</v>
       </c>
@@ -812,7 +807,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>9</v>
       </c>
@@ -836,12 +831,12 @@
       <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -852,7 +847,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -863,7 +858,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -874,7 +869,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -885,7 +880,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -896,7 +891,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -907,7 +902,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -918,7 +913,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -929,7 +924,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -940,7 +935,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -951,7 +946,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -962,7 +957,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -973,7 +968,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -984,7 +979,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -995,7 +990,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -1006,7 +1001,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -1017,7 +1012,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -1028,7 +1023,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -1039,7 +1034,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -1050,7 +1045,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>5</v>
       </c>
@@ -1061,7 +1056,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>5</v>
       </c>
@@ -1072,7 +1067,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>5</v>
       </c>
@@ -1083,7 +1078,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -1094,7 +1089,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -1105,7 +1100,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -1116,7 +1111,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>8</v>
       </c>
@@ -1127,7 +1122,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>8</v>
       </c>
@@ -1138,7 +1133,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>8</v>
       </c>
@@ -1149,7 +1144,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>8</v>
       </c>
@@ -1160,7 +1155,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>9</v>
       </c>
@@ -1171,7 +1166,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>9</v>
       </c>
@@ -1182,7 +1177,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>9</v>
       </c>
@@ -1193,7 +1188,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>9</v>
       </c>
@@ -1204,7 +1199,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>9</v>
       </c>
@@ -1215,7 +1210,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>9</v>
       </c>
@@ -1226,7 +1221,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>9</v>
       </c>
@@ -1237,7 +1232,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>7</v>
       </c>
@@ -1248,7 +1243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>7</v>
       </c>
@@ -1259,7 +1254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>7</v>
       </c>
@@ -1270,7 +1265,7 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>7</v>
       </c>
@@ -1281,7 +1276,7 @@
         <v>-15</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>7</v>
       </c>
@@ -1292,7 +1287,7 @@
         <v>-23</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>7</v>
       </c>
@@ -1303,7 +1298,7 @@
         <v>-44</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
Re-change Prognos input data back
it was said to include not only ROR, but also reservoir
</commit_message>
<xml_diff>
--- a/raw_data_input/renewables/Prognos_et_al_2020_RES_data.xlsx
+++ b/raw_data_input/renewables/Prognos_et_al_2020_RES_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\koch_j0\POMMES_public\pommes-data\raw_data_input\renewables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A0F28E0-F665-4E55-A1EF-4D11C9AF3C71}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DE6785F-B088-40A8-A894-9148F7266C62}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" xr2:uid="{5D64F573-EFB4-433D-A285-0A55FC20DE65}"/>
   </bookViews>
@@ -58,7 +58,7 @@
     <t>biomassEEG</t>
   </si>
   <si>
-    <t>ROR</t>
+    <t>Wasser</t>
   </si>
 </sst>
 </file>
@@ -413,7 +413,7 @@
   <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:A29"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>